<commit_message>
Redesigend UI, fixed some minor Live Editor bugs
</commit_message>
<xml_diff>
--- a/ExcelData/BATCH_TEST_Batch.xlsx
+++ b/ExcelData/BATCH_TEST_Batch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\UE4_Shloc_Suite\ShlocToolsSuite\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UE4_Projects\UE4_Shloc_Suite\ShlocToolsSuite\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44A075A-1D9F-40A2-9FF1-81DDE8FABA03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C77BC1-7508-4140-9E5A-E6019BCC4361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27360" yWindow="4545" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopText" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Key</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>HELLO</t>
-  </si>
-  <si>
     <t>TextData_ShopText_Text_SHOP_ITEM_BUY_DLG_CANCEL_SLCT</t>
   </si>
   <si>
@@ -40,10 +37,34 @@
     <t>longest_name</t>
   </si>
   <si>
+    <t>TextID</t>
+  </si>
+  <si>
+    <t>年会</t>
+  </si>
+  <si>
+    <t>SwordOfTruth_Price</t>
+  </si>
+  <si>
+    <t>190 gold</t>
+  </si>
+  <si>
+    <t>長出</t>
+  </si>
+  <si>
+    <t>BattleText_TagTest</t>
+  </si>
+  <si>
     <t>battle_text</t>
   </si>
   <si>
-    <t>battle_text HELLO longest_name HELLO</t>
+    <t>battle_text longest_name</t>
+  </si>
+  <si>
+    <t>Multiple_TagTest</t>
+  </si>
+  <si>
+    <t>LongestName_TagTest</t>
   </si>
 </sst>
 </file>
@@ -884,68 +905,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of new changes
</commit_message>
<xml_diff>
--- a/ExcelData/BATCH_TEST_Batch.xlsx
+++ b/ExcelData/BATCH_TEST_Batch.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UE4_Projects\UE4_Shloc_Suite\ShlocToolsSuite\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C77BC1-7508-4140-9E5A-E6019BCC4361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23F032A-9DEA-40B9-A1DE-17F4A9696170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27360" yWindow="4545" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2985" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopText" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Key</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>LongestName_TagTest</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>WWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWW</t>
+  </si>
+  <si>
+    <t>36Ws</t>
   </si>
 </sst>
 </file>
@@ -905,16 +914,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
@@ -988,6 +997,39 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
need to QA batch checker but mostly done
</commit_message>
<xml_diff>
--- a/ExcelData/BATCH_TEST_Batch.xlsx
+++ b/ExcelData/BATCH_TEST_Batch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UE4_Projects\UE4_Shloc_Suite\ShlocToolsSuite\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C705DF4-016F-41AE-9E3A-BEDA15A811A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEA5941-B7A3-4B8E-B65C-1DD4689F37A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8790" yWindow="3960" windowWidth="28800" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopText" sheetId="1" r:id="rId1"/>
@@ -67,13 +67,13 @@
     <t>長出 TEST</t>
   </si>
   <si>
-    <t>WITCH</t>
-  </si>
-  <si>
     <t>MaxWs</t>
   </si>
   <si>
-    <t>WWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWW</t>
+    <t>W_TEST</t>
+  </si>
+  <si>
+    <t>WWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWWW</t>
   </si>
 </sst>
 </file>
@@ -917,21 +917,21 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.26953125" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -953,7 +953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -964,7 +964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -975,7 +975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -986,7 +986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -997,15 +997,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>